<commit_message>
server list test case added
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/login/login - password_field.xlsx
+++ b/apps/features/backlog/desktop/windows/login/login - password_field.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\login\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8221970-DFFF-4F33-B0EF-DDB7BE354526}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB37AC6-E0E4-4521-AE23-6F5E73500505}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1515,7 +1515,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>